<commit_message>
Eliminar archivos de prueba obsoletos y agregar nuevas implementaciones para la gestión de agentes y recompensas en el entorno multi-agente.
</commit_message>
<xml_diff>
--- a/training_results.xlsx
+++ b/training_results.xlsx
@@ -418,13 +418,13 @@
         <v>0</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>2800.36962890625</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>6339.204658508301</v>
       </c>
       <c r="H2">
-        <v>0</v>
+        <v>-0.00144983336358564</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -444,13 +444,13 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>2038.646362304688</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>3842.476371383667</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>-0.004288706836814526</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -470,13 +470,13 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>2232.480224609375</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>4872.34213104248</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-0.006103016252745874</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -496,13 +496,13 @@
         <v>0</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>937.7421264648438</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>2071.899267101288</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>-0.0006716600968502462</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -522,13 +522,13 @@
         <v>0</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1573.872436523438</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>2467.002140808106</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>-0.00499326687422581</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -548,13 +548,13 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>864.0095825195312</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>1688.926021671295</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>-0.01041941584990127</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -574,13 +574,13 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1099.135375976562</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>1726.232862663269</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>-0.00616969806724228</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -600,13 +600,13 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>1107.322387695312</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2159.704662322998</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>-0.003283517652016599</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -626,13 +626,13 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1264.18701171875</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>2584.118773269654</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>-0.003561254777014256</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -652,13 +652,13 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>1826.040161132812</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>3017.28395023346</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>-0.004216554155573249</v>
       </c>
     </row>
     <row r="12" spans="1:8">
@@ -678,13 +678,13 @@
         <v>0</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>4355.26416015625</v>
       </c>
       <c r="G12">
-        <v>0</v>
+        <v>10947.3561920166</v>
       </c>
       <c r="H12">
-        <v>0</v>
+        <v>-0.0008711992559256032</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -704,13 +704,13 @@
         <v>0</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>4838.90966796875</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>10701.12629089356</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>-0.002393631459563039</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -730,13 +730,13 @@
         <v>0</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>2932.761474609375</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>6351.350623321533</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>-0.004734256540541537</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -756,13 +756,13 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>5786.4560546875</v>
       </c>
       <c r="G15">
-        <v>0</v>
+        <v>12678.13593139648</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>-0.00145573744957801</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -782,13 +782,13 @@
         <v>0</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>7655.37255859375</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>15839.49108886719</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>-0.001733577916456852</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -808,13 +808,13 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>6597.56689453125</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>13701.03952331543</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>-0.0001805321458959952</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -834,13 +834,13 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>7282.2412109375</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>14670.90635681152</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>-0.002791798187536187</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -860,13 +860,13 @@
         <v>0</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>7418.810546875</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>15974.66792602539</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>-0.004707348303054459</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -886,13 +886,13 @@
         <v>0</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>8097.8779296875</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>16882.61979980469</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>-0.004683819354249863</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -912,13 +912,13 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>7715.57080078125</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>16396.66737365723</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>-0.003791472605371382</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -938,13 +938,13 @@
         <v>0</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>7934.7939453125</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>16373.1244354248</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>-0.003560015169205144</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -964,13 +964,13 @@
         <v>0</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>7975.16357421875</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>16736.23780517578</v>
       </c>
       <c r="H23">
-        <v>0</v>
+        <v>-0.002663144693360664</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -990,13 +990,13 @@
         <v>0</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>7701.09765625</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>16211.25744628906</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>-0.001943372350069694</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1016,13 +1016,13 @@
         <v>0</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>7724.21533203125</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>15956.39193115234</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>-0.002322121861470805</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1042,13 +1042,13 @@
         <v>0</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>7637.8779296875</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>15778.47079467773</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>-0.001156363797781523</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1068,13 +1068,13 @@
         <v>0</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>7765.42919921875</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>15856.32176513672</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>-0.003244193001592066</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1094,13 +1094,13 @@
         <v>0</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>7290.9609375</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>15295.15351867676</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>-0.0006269599609368016</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1120,13 +1120,13 @@
         <v>0</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>7097.7783203125</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>14791.36311645508</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>-0.001980978442588821</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1146,13 +1146,13 @@
         <v>0</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>6952.54345703125</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>14689.16779174805</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>-0.002578061895474093</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1172,13 +1172,13 @@
         <v>0</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>6718.5537109375</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>14141.06915283203</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>-0.003381397216435289</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -1198,13 +1198,13 @@
         <v>0</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>6473.56591796875</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>13543.2236114502</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>-0.001699616969563067</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1224,13 +1224,13 @@
         <v>0</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>6273.94189453125</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>13946.93997497559</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>-0.0001685482857283205</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -1250,13 +1250,13 @@
         <v>0</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>6311.078125</v>
       </c>
       <c r="G34">
-        <v>0</v>
+        <v>13525.97136535644</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>-0.0007269616100529675</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -1276,13 +1276,13 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>6460.1875</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>13532.21586608887</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>-0.0008376329264137894</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1302,13 +1302,13 @@
         <v>0</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>6047.34912109375</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>12867.80270385742</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>-0.002197616519697476</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -1328,13 +1328,13 @@
         <v>0</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>5912.4873046875</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>12597.45914306641</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>-0.00136258380007348</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -1354,13 +1354,13 @@
         <v>0</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>5435.591796875</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>11577.05453491211</v>
       </c>
       <c r="H38">
-        <v>0</v>
+        <v>-0.002807083747757133</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1380,13 +1380,13 @@
         <v>0</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>5148.28466796875</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>11177.20144348144</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>-0.0004798017609573435</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1406,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>4110.724609375</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>9055.592010498047</v>
       </c>
       <c r="H40">
-        <v>0</v>
+        <v>-0.00562450872057525</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1432,13 +1432,13 @@
         <v>0</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>4681.67919921875</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>9981.099282836914</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>8.614140751888044E-05</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1458,13 +1458,13 @@
         <v>0</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>5035.5224609375</v>
       </c>
       <c r="G42">
-        <v>0</v>
+        <v>10682.61312255859</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>-0.001666768560244236</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1484,13 +1484,13 @@
         <v>0</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>4617.8857421875</v>
       </c>
       <c r="G43">
-        <v>0</v>
+        <v>9793.310021972657</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>-0.001639774674549699</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1510,13 +1510,13 @@
         <v>0</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>4795.81298828125</v>
       </c>
       <c r="G44">
-        <v>0</v>
+        <v>10572.38519592285</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>-0.004111758900398855</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1536,13 +1536,13 @@
         <v>0</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>5223.08740234375</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>10977.60778503418</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>-0.002324502915143967</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1562,13 +1562,13 @@
         <v>0</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>4920.59375</v>
       </c>
       <c r="G46">
-        <v>0</v>
+        <v>10682.0315246582</v>
       </c>
       <c r="H46">
-        <v>0</v>
+        <v>-0.001567116061050911</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1588,13 +1588,13 @@
         <v>0</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>4243.64453125</v>
       </c>
       <c r="G47">
-        <v>0</v>
+        <v>9010.626727294923</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>-0.001670904037746368</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -1614,13 +1614,13 @@
         <v>0</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>3541.82373046875</v>
       </c>
       <c r="G48">
-        <v>0</v>
+        <v>7807.113577270507</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>-0.001626361085800454</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -1640,13 +1640,13 @@
         <v>0</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>3790.680908203125</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>8220.167330932618</v>
       </c>
       <c r="H49">
-        <v>0</v>
+        <v>-0.000961233135603834</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -1666,13 +1666,13 @@
         <v>0</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>4198.04052734375</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>8724.015969848633</v>
       </c>
       <c r="H50">
-        <v>0</v>
+        <v>-0.002133967486588517</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -1692,13 +1692,13 @@
         <v>0</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>4267.3232421875</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>9369.511758422852</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>-5.379499052651227E-05</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -1718,13 +1718,13 @@
         <v>0</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>4196.0009765625</v>
       </c>
       <c r="G52">
-        <v>0</v>
+        <v>8924.833955383301</v>
       </c>
       <c r="H52">
-        <v>0</v>
+        <v>-0.0007870839443057775</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -1744,13 +1744,13 @@
         <v>0</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>3618.954833984375</v>
       </c>
       <c r="G53">
-        <v>0</v>
+        <v>7892.889468383789</v>
       </c>
       <c r="H53">
-        <v>0</v>
+        <v>-0.001694243446399923</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -1770,13 +1770,13 @@
         <v>0</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>4069.03759765625</v>
       </c>
       <c r="G54">
-        <v>0</v>
+        <v>8412.899340820313</v>
       </c>
       <c r="H54">
-        <v>0</v>
+        <v>2.813310929923318E-05</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -1796,13 +1796,13 @@
         <v>0</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>3773.9755859375</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>8496.234910583496</v>
       </c>
       <c r="H55">
-        <v>0</v>
+        <v>-0.004859730902535375</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -1822,13 +1822,13 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>3081.41455078125</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>6790.056242370605</v>
       </c>
       <c r="H56">
-        <v>0</v>
+        <v>0.0005491443640494254</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -1848,13 +1848,13 @@
         <v>0</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>3126.74951171875</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>6656.116520690918</v>
       </c>
       <c r="H57">
-        <v>0</v>
+        <v>-0.001026444463059306</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -1874,13 +1874,13 @@
         <v>0</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>2024.9169921875</v>
       </c>
       <c r="G58">
-        <v>0</v>
+        <v>3760.90966873169</v>
       </c>
       <c r="H58">
-        <v>0</v>
+        <v>-0.006091473050764762</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -1900,13 +1900,13 @@
         <v>0</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>287.4891357421875</v>
       </c>
       <c r="G59">
-        <v>0</v>
+        <v>848.4966359138489</v>
       </c>
       <c r="H59">
-        <v>0</v>
+        <v>-0.0009344543068436906</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -1926,13 +1926,13 @@
         <v>0</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>1062.641357421875</v>
       </c>
       <c r="G60">
-        <v>0</v>
+        <v>2859.101824951172</v>
       </c>
       <c r="H60">
-        <v>0</v>
+        <v>-0.0009905669547151774</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -1952,13 +1952,13 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>394.4233703613281</v>
       </c>
       <c r="G61">
-        <v>0</v>
+        <v>1204.947859477997</v>
       </c>
       <c r="H61">
-        <v>0</v>
+        <v>-0.005540395886055194</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -1978,13 +1978,13 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>2392.587158203125</v>
       </c>
       <c r="G62">
-        <v>0</v>
+        <v>4952.652317047119</v>
       </c>
       <c r="H62">
-        <v>0</v>
+        <v>-0.000189485122973565</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2004,13 +2004,13 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>2292.50341796875</v>
       </c>
       <c r="G63">
-        <v>0</v>
+        <v>5150.986410522461</v>
       </c>
       <c r="H63">
-        <v>0</v>
+        <v>-0.002049886548775248</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2030,13 +2030,13 @@
         <v>0</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>1672.58349609375</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>3452.872358703613</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>-0.0024824301188346</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2056,13 +2056,13 @@
         <v>0</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>360.3073425292969</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>1068.969723701477</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>-0.003118606185307726</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2082,13 +2082,13 @@
         <v>0</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>243.0913543701172</v>
       </c>
       <c r="G66">
-        <v>0</v>
+        <v>776.0960458278656</v>
       </c>
       <c r="H66">
-        <v>0</v>
+        <v>-0.001686850131954998</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2108,13 +2108,13 @@
         <v>0</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>262.1437377929688</v>
       </c>
       <c r="G67">
-        <v>0</v>
+        <v>500.2911525726319</v>
       </c>
       <c r="H67">
-        <v>0</v>
+        <v>-0.003464404330588877</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2134,13 +2134,13 @@
         <v>0</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>97.72964477539062</v>
       </c>
       <c r="G68">
-        <v>0</v>
+        <v>369.4734858840704</v>
       </c>
       <c r="H68">
-        <v>0</v>
+        <v>-0.002226909513410646</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2160,13 +2160,13 @@
         <v>0</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>44.87535095214844</v>
       </c>
       <c r="G69">
-        <v>0</v>
+        <v>212.9398467727005</v>
       </c>
       <c r="H69">
-        <v>0</v>
+        <v>-0.0003930538019631058</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -2186,13 +2186,13 @@
         <v>0</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>121.9629592895508</v>
       </c>
       <c r="G70">
-        <v>0</v>
+        <v>212.3798038490117</v>
       </c>
       <c r="H70">
-        <v>0</v>
+        <v>-0.0002487653386197053</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -2212,13 +2212,13 @@
         <v>0</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>214.6184997558594</v>
       </c>
       <c r="G71">
-        <v>0</v>
+        <v>429.015706477128</v>
       </c>
       <c r="H71">
-        <v>0</v>
+        <v>-0.001295065713929944</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -2238,13 +2238,13 @@
         <v>0</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>116.8886566162109</v>
       </c>
       <c r="G72">
-        <v>0</v>
+        <v>252.4195757318288</v>
       </c>
       <c r="H72">
-        <v>0</v>
+        <v>-0.0005901276046643034</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -2264,13 +2264,13 @@
         <v>0</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>120.8513336181641</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>266.080407717824</v>
       </c>
       <c r="H73">
-        <v>0</v>
+        <v>-0.00016262570861727</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -2290,13 +2290,13 @@
         <v>0</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>217.3560943603516</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>162.7646819068119</v>
       </c>
       <c r="H74">
-        <v>0</v>
+        <v>6.706359272357076E-06</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -2316,13 +2316,13 @@
         <v>0</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>180.6278839111328</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>580.017489361763</v>
       </c>
       <c r="H75">
-        <v>0</v>
+        <v>-0.004401172974030487</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -2342,13 +2342,13 @@
         <v>0</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>87.11888122558594</v>
       </c>
       <c r="G76">
-        <v>0</v>
+        <v>276.6670676492155</v>
       </c>
       <c r="H76">
-        <v>0</v>
+        <v>-0.002371813479112461</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -2368,13 +2368,13 @@
         <v>0</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>189.2112121582031</v>
       </c>
       <c r="G77">
-        <v>0</v>
+        <v>187.22485322766</v>
       </c>
       <c r="H77">
-        <v>0</v>
+        <v>0.0002765461038507056</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -2394,13 +2394,13 @@
         <v>0</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>59.45317459106445</v>
       </c>
       <c r="G78">
-        <v>0</v>
+        <v>121.7740472955629</v>
       </c>
       <c r="H78">
-        <v>0</v>
+        <v>-0.0002325933179236017</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -2420,13 +2420,13 @@
         <v>0</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>55.14452362060547</v>
       </c>
       <c r="G79">
-        <v>0</v>
+        <v>255.8233480532654</v>
       </c>
       <c r="H79">
-        <v>0</v>
+        <v>0.0002640176433487795</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -2446,13 +2446,13 @@
         <v>0</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>110.2554626464844</v>
       </c>
       <c r="G80">
-        <v>0</v>
+        <v>174.9530838417821</v>
       </c>
       <c r="H80">
-        <v>0</v>
+        <v>0.00130901294760406</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -2472,13 +2472,13 @@
         <v>0</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>76.52084350585938</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>149.7140434024855</v>
       </c>
       <c r="H81">
-        <v>0</v>
+        <v>-0.0003523349165334366</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -2498,13 +2498,13 @@
         <v>0</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>23.31660079956055</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>115.002769084461</v>
       </c>
       <c r="H82">
-        <v>0</v>
+        <v>-0.002128286388324341</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -2524,13 +2524,13 @@
         <v>0</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>97.010009765625</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>198.4828403848223</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>-6.047480128472671E-05</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -2550,13 +2550,13 @@
         <v>0</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>71.12770843505859</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>320.6329550629482</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>0.001331211331125814</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -2576,13 +2576,13 @@
         <v>0</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>117.4766159057617</v>
       </c>
       <c r="G85">
-        <v>0</v>
+        <v>333.2028957651928</v>
       </c>
       <c r="H85">
-        <v>0</v>
+        <v>-0.002373785026429687</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -2602,13 +2602,13 @@
         <v>0</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>70.75559997558594</v>
       </c>
       <c r="G86">
-        <v>0</v>
+        <v>251.9764899048954</v>
       </c>
       <c r="H86">
-        <v>0</v>
+        <v>0.0003883952529577073</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -2628,13 +2628,13 @@
         <v>0</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>29.70674705505371</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>132.2928648229689</v>
       </c>
       <c r="H87">
-        <v>0</v>
+        <v>-0.002535645811076392</v>
       </c>
     </row>
     <row r="88" spans="1:8">
@@ -2654,13 +2654,13 @@
         <v>0</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>36.95839309692383</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>137.0266237122007</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>0.0001562636709422804</v>
       </c>
     </row>
     <row r="89" spans="1:8">
@@ -2680,13 +2680,13 @@
         <v>0</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>5.892275810241699</v>
       </c>
       <c r="G89">
-        <v>0</v>
+        <v>105.1565341127105</v>
       </c>
       <c r="H89">
-        <v>0</v>
+        <v>0.0007242407271405682</v>
       </c>
     </row>
     <row r="90" spans="1:8">
@@ -2706,13 +2706,13 @@
         <v>0</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>34.63279724121094</v>
       </c>
       <c r="G90">
-        <v>0</v>
+        <v>93.29019634760917</v>
       </c>
       <c r="H90">
-        <v>0</v>
+        <v>0.0002293591927809757</v>
       </c>
     </row>
     <row r="91" spans="1:8">
@@ -2732,13 +2732,13 @@
         <v>0</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>54.42511367797852</v>
       </c>
       <c r="G91">
-        <v>0</v>
+        <v>128.3450532611459</v>
       </c>
       <c r="H91">
-        <v>0</v>
+        <v>-0.004455352104560007</v>
       </c>
     </row>
     <row r="92" spans="1:8">
@@ -2758,13 +2758,13 @@
         <v>0</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>0.2418511658906937</v>
       </c>
       <c r="G92">
-        <v>0</v>
+        <v>33.15821650647558</v>
       </c>
       <c r="H92">
-        <v>0</v>
+        <v>-0.00178755702872877</v>
       </c>
     </row>
     <row r="93" spans="1:8">
@@ -2784,13 +2784,13 @@
         <v>0</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>48.54049682617188</v>
       </c>
       <c r="G93">
-        <v>0</v>
+        <v>25.35009117776062</v>
       </c>
       <c r="H93">
-        <v>0</v>
+        <v>-0.0006232345513126347</v>
       </c>
     </row>
     <row r="94" spans="1:8">
@@ -2810,13 +2810,13 @@
         <v>0</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>5.564521312713623</v>
       </c>
       <c r="G94">
-        <v>0</v>
+        <v>10.62352459498215</v>
       </c>
       <c r="H94">
-        <v>0</v>
+        <v>0.0004065224704390857</v>
       </c>
     </row>
     <row r="95" spans="1:8">
@@ -2836,13 +2836,13 @@
         <v>0</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>0.5109555721282959</v>
       </c>
       <c r="G95">
-        <v>0</v>
+        <v>14.14626812809147</v>
       </c>
       <c r="H95">
-        <v>0</v>
+        <v>-0.004212537832790986</v>
       </c>
     </row>
     <row r="96" spans="1:8">
@@ -2862,13 +2862,13 @@
         <v>0</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>0.28370600938797</v>
       </c>
       <c r="G96">
-        <v>0</v>
+        <v>11.85763699216768</v>
       </c>
       <c r="H96">
-        <v>0</v>
+        <v>-0.0007580308898468502</v>
       </c>
     </row>
     <row r="97" spans="1:8">
@@ -2888,13 +2888,13 @@
         <v>0</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>2.35822606086731</v>
       </c>
       <c r="G97">
-        <v>0</v>
+        <v>3.79584109801799</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>-7.347779501287732E-05</v>
       </c>
     </row>
     <row r="98" spans="1:8">
@@ -2914,13 +2914,13 @@
         <v>0</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>0.1274566352367401</v>
       </c>
       <c r="G98">
-        <v>0</v>
+        <v>7.283154574106447</v>
       </c>
       <c r="H98">
-        <v>0</v>
+        <v>0.001543968964688247</v>
       </c>
     </row>
     <row r="99" spans="1:8">
@@ -2940,13 +2940,13 @@
         <v>0</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>0.2174239456653595</v>
       </c>
       <c r="G99">
-        <v>0</v>
+        <v>3.077484695822932</v>
       </c>
       <c r="H99">
-        <v>0</v>
+        <v>-0.000759537833801005</v>
       </c>
     </row>
     <row r="100" spans="1:8">
@@ -2966,13 +2966,13 @@
         <v>0</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>0.4579973816871643</v>
       </c>
       <c r="G100">
-        <v>0</v>
+        <v>1.667394351761323</v>
       </c>
       <c r="H100">
-        <v>0</v>
+        <v>0.001068112662687781</v>
       </c>
     </row>
     <row r="101" spans="1:8">
@@ -2992,13 +2992,13 @@
         <v>0</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>5.769603252410889</v>
       </c>
       <c r="G101">
-        <v>0</v>
+        <v>1.843379506655037</v>
       </c>
       <c r="H101">
-        <v>0</v>
+        <v>-0.002376615070534172</v>
       </c>
     </row>
   </sheetData>

</xml_diff>